<commit_message>
Tested first smspp builder
Integrated succesfully get as dense to take into account snapshot weightings.
- Handle lines (their size with L*T)
- Test the other cases and components
</commit_message>
<xml_diff>
--- a/data/components.xlsx
+++ b/data/components.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\smspp-project\PyPSA_SMS_interface\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\smspp-project\transformation_pypsa_smspp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>solar</t>
   </si>
@@ -183,7 +183,13 @@
     <t>p_nom_max</t>
   </si>
   <si>
-    <t>diesel 1</t>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>onwind</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,6 +603,14 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
     </row>
@@ -795,14 +809,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
@@ -839,7 +853,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
@@ -854,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -862,7 +876,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>37</v>
@@ -874,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -942,10 +956,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,6 +1004,32 @@
         <v>36</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.95</v>
+      </c>
+      <c r="G2">
+        <v>0.95</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tested with 1N and 2N
What does not work
1- hydro
2- hydro as battery (negative power)
3- error of 0.5% to be analysed (main script, 1 line, 1 wind, 1 diesel, 1 battery)
</commit_message>
<xml_diff>
--- a/data/components.xlsx
+++ b/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +693,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +744,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,7 +810,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -958,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Inverse transformation - up to thermal
Tested with multiple
ThermalUnitBlocks
BatteryUnitBlocks
IntermittentUnitBlocks

Still to add lines and hydro generators
</commit_message>
<xml_diff>
--- a/data/components.xlsx
+++ b/data/components.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>solar</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>battery_link</t>
+  </si>
+  <si>
+    <t>line_0-1</t>
+  </si>
+  <si>
+    <t>diesel</t>
   </si>
 </sst>
 </file>
@@ -746,10 +752,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,6 +788,29 @@
         <v>40</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -789,10 +818,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,6 +882,29 @@
         <v>150</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -860,10 +912,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,34 +953,6 @@
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>